<commit_message>
Fixed problems with mergeSort algorithm, refreshed diagrams to represent new values.
</commit_message>
<xml_diff>
--- a/TL_Feladat04/Diagramok.xlsx
+++ b/TL_Feladat04/Diagramok.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="12">
   <si>
     <t>Algoritmus</t>
   </si>
@@ -160,7 +157,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="hu-HU" baseline="0"/>
-              <a:t> összehasonlítása</a:t>
+              <a:t> összehasonlítása nagyobb adathalmaznál</a:t>
             </a:r>
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
@@ -230,54 +227,78 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Munka1!$B$2:$B$7</c:f>
+              <c:f>Munka1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1000</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5000</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10000</c:v>
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Munka1!$H$2:$H$7</c:f>
+              <c:f>Munka1!$H$2:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>54.6</c:v>
+                  <c:v>9.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45.8</c:v>
+                  <c:v>52.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.8</c:v>
+                  <c:v>98.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>119.8</c:v>
+                  <c:v>439.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>423.6</c:v>
+                  <c:v>808.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>826</c:v>
+                  <c:v>5022.6000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10375.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59202</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>122156.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>249535</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -293,15 +314,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Munka1!$A$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Paralell Merge Sort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Paralell Merge Sort min 10000</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -317,54 +330,78 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Munka1!$B$20:$B$25</c:f>
+              <c:f>Munka1!$B$22:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1000</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5000</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10000</c:v>
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Munka1!$H$20:$H$25</c:f>
+              <c:f>Munka1!$H$22:$H$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>229.8</c:v>
+                  <c:v>19.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>145.19999999999999</c:v>
+                  <c:v>109.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>541.6</c:v>
+                  <c:v>259.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>738.4</c:v>
+                  <c:v>1255.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13971.8</c:v>
+                  <c:v>3177.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40681.199999999997</c:v>
+                  <c:v>5594.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8341.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36940.199999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80185.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>148679.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -373,6 +410,109 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-7A14-4C32-8300-F3F0E8C22EBF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Paralell Merge Sort min 1000</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Munka1!$B$12:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Munka1!$H$12:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>102.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>356.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>797.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2045.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4053</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8073.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47634.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81040.800000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>159092.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6864-4566-919B-54C9DF2771C3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -770,7 +910,18 @@
               <a:rPr lang="hu-HU" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Paralell Merge Sort különböző minimális egy szálon futtatott tömbmérettel</a:t>
+              <a:t>Paralell Merge Sort különböző minimális egy szálon futtatott tömbmérettel </a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="hu-HU" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+            </a:br>
+            <a:r>
+              <a:rPr lang="hu-HU" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(2 000 000 méretű tömbnél)</a:t>
             </a:r>
             <a:endParaRPr lang="hu-HU" sz="1400">
               <a:effectLst/>
@@ -837,36 +988,36 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>(Munka1!$I$8,Munka1!$I$14,Munka1!$I$20)</c:f>
+              <c:f>(Munka1!$I$21,Munka1!$I$31,Munka1!$I$41)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>500</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Munka1!$H$11,Munka1!$H$17,Munka1!$H$23)</c:f>
+              <c:f>(Munka1!$H$21,Munka1!$H$31,Munka1!$H$41)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5057</c:v>
+                  <c:v>159092.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1376.4</c:v>
+                  <c:v>148679.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>738.4</c:v>
+                  <c:v>145050.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1220,6 +1371,689 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="hu-HU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hu-HU"/>
+              <a:t>Algoritmusok</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="hu-HU" baseline="0"/>
+              <a:t> összehasonlítása kisebb adathalmaznál</a:t>
+            </a:r>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Munka1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Munka1!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Munka1!$H$2:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>439.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>808.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5022.6000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4634-4D1D-89F5-A69A9D641547}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Paralell Merge Sort min 10000</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Munka1!$B$22:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Munka1!$H$22:$H$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>19.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>109.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>259.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1255.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3177.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5594.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4634-4D1D-89F5-A69A9D641547}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Paralell Merge Sort min 1000</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Munka1!$B$12:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Munka1!$H$12:$H$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>102.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>356.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>797.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2045.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4053</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4634-4D1D-89F5-A69A9D641547}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="551921471"/>
+        <c:axId val="551919391"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="551921471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU" sz="1200"/>
+                  <a:t>Méret</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="551919391"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="551919391"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU" sz="1200" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Idő (µs)</a:t>
+                </a:r>
+                <a:endParaRPr lang="hu-HU" sz="700">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="551921471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="hu-HU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1300,6 +2134,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2300,6 +3174,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2324,14 +3714,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:colOff>600074</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2355,13 +3745,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2381,142 +3771,39 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Diagram 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Munka1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>Quick Sort</v>
-          </cell>
-          <cell r="B2">
-            <v>100</v>
-          </cell>
-          <cell r="H2">
-            <v>941</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>500</v>
-          </cell>
-          <cell r="H3">
-            <v>1049.5999999999999</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>1000</v>
-          </cell>
-          <cell r="H4">
-            <v>1213</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>5000</v>
-          </cell>
-          <cell r="H5">
-            <v>2439.1999999999998</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>10000</v>
-          </cell>
-          <cell r="H6">
-            <v>6063</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>50000</v>
-          </cell>
-          <cell r="H7">
-            <v>20973.8</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="H10">
-            <v>502779</v>
-          </cell>
-          <cell r="I10">
-            <v>100</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="H16">
-            <v>3233.4</v>
-          </cell>
-          <cell r="I16">
-            <v>1000</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>Paralell Merge Sort</v>
-          </cell>
-          <cell r="B20">
-            <v>100</v>
-          </cell>
-          <cell r="H20">
-            <v>1392.2</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>500</v>
-          </cell>
-          <cell r="H21">
-            <v>1725.4</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22">
-            <v>1000</v>
-          </cell>
-          <cell r="H22">
-            <v>2531.8000000000002</v>
-          </cell>
-          <cell r="I22">
-            <v>5000</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23">
-            <v>5000</v>
-          </cell>
-          <cell r="H23">
-            <v>6937</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24">
-            <v>10000</v>
-          </cell>
-          <cell r="H24">
-            <v>255644</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25">
-            <v>50000</v>
-          </cell>
-          <cell r="H25">
-            <v>480981</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2782,15 +4069,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2831,23 +4119,23 @@
         <v>100</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="D2">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E2">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="F2">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="G2">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="H2">
-        <f>AVERAGE(C2:G2)</f>
-        <v>54.6</v>
+        <f t="shared" ref="H2:H43" si="0">AVERAGE(C2:G2)</f>
+        <v>9.4</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
@@ -2858,26 +4146,26 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="C3">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="D3">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="E3">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F3">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="G3">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H25" si="0">AVERAGE(C3:G3)</f>
-        <v>45.8</v>
+        <f t="shared" si="0"/>
+        <v>52.4</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
@@ -2888,26 +4176,26 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="C4">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="D4">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="E4">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="F4">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="G4">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>71.8</v>
+        <v>98.6</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
@@ -2918,26 +4206,26 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="C5">
-        <v>110</v>
+        <v>363</v>
       </c>
       <c r="D5">
-        <v>112</v>
+        <v>673</v>
       </c>
       <c r="E5">
-        <v>108</v>
+        <v>386</v>
       </c>
       <c r="F5">
-        <v>119</v>
+        <v>394</v>
       </c>
       <c r="G5">
-        <v>150</v>
+        <v>383</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>119.8</v>
+        <v>439.8</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
@@ -2948,26 +4236,26 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="C6">
-        <v>647</v>
+        <v>792</v>
       </c>
       <c r="D6">
-        <v>381</v>
+        <v>801</v>
       </c>
       <c r="E6">
-        <v>360</v>
+        <v>793</v>
       </c>
       <c r="F6">
-        <v>360</v>
+        <v>845</v>
       </c>
       <c r="G6">
-        <v>370</v>
+        <v>810</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>423.6</v>
+        <v>808.2</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
@@ -2978,26 +4266,26 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="C7">
-        <v>841</v>
+        <v>4640</v>
       </c>
       <c r="D7">
-        <v>863</v>
+        <v>5561</v>
       </c>
       <c r="E7">
-        <v>810</v>
+        <v>5270</v>
       </c>
       <c r="F7">
-        <v>768</v>
+        <v>4682</v>
       </c>
       <c r="G7">
-        <v>848</v>
+        <v>4960</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>826</v>
+        <v>5022.6000000000004</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
@@ -3005,122 +4293,122 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="C8">
-        <v>314</v>
+        <v>10869</v>
       </c>
       <c r="D8">
-        <v>145</v>
+        <v>9912</v>
       </c>
       <c r="E8">
-        <v>146</v>
+        <v>10386</v>
       </c>
       <c r="F8">
-        <v>118</v>
+        <v>10652</v>
       </c>
       <c r="G8">
-        <v>114</v>
+        <v>10059</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>167.4</v>
-      </c>
-      <c r="I8">
-        <v>100</v>
+        <v>10375.6</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9">
-        <v>200</v>
+        <v>500000</v>
       </c>
       <c r="C9">
-        <v>614</v>
+        <v>57395</v>
       </c>
       <c r="D9">
-        <v>502</v>
+        <v>56756</v>
       </c>
       <c r="E9">
-        <v>373</v>
+        <v>63151</v>
       </c>
       <c r="F9">
-        <v>370</v>
+        <v>58011</v>
       </c>
       <c r="G9">
-        <v>391</v>
+        <v>60697</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>450</v>
-      </c>
-      <c r="I9">
-        <v>100</v>
+        <v>59202</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>500</v>
+        <v>1000000</v>
       </c>
       <c r="C10">
-        <v>1735</v>
+        <v>123305</v>
       </c>
       <c r="D10">
-        <v>1366</v>
+        <v>121115</v>
       </c>
       <c r="E10">
-        <v>1062</v>
+        <v>120097</v>
       </c>
       <c r="F10">
-        <v>1895</v>
+        <v>124256</v>
       </c>
       <c r="G10">
-        <v>2500</v>
+        <v>122008</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>1711.6</v>
-      </c>
-      <c r="I10">
-        <v>100</v>
+        <v>122156.2</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11">
-        <v>1000</v>
+        <v>2000000</v>
       </c>
       <c r="C11">
-        <v>3588</v>
+        <v>251304</v>
       </c>
       <c r="D11">
-        <v>3506</v>
+        <v>250318</v>
       </c>
       <c r="E11">
-        <v>5326</v>
+        <v>248144</v>
       </c>
       <c r="F11">
-        <v>8186</v>
+        <v>250724</v>
       </c>
       <c r="G11">
-        <v>4679</v>
+        <v>247185</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>5057</v>
-      </c>
-      <c r="I11">
-        <v>100</v>
+        <v>249535</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3128,29 +4416,29 @@
         <v>3</v>
       </c>
       <c r="B12">
-        <v>5000</v>
+        <v>100</v>
       </c>
       <c r="C12">
-        <v>29142</v>
+        <v>111</v>
       </c>
       <c r="D12">
-        <v>19958</v>
+        <v>123</v>
       </c>
       <c r="E12">
-        <v>20605</v>
+        <v>100</v>
       </c>
       <c r="F12">
-        <v>25789</v>
+        <v>92</v>
       </c>
       <c r="G12">
-        <v>25096</v>
+        <v>85</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>24118</v>
-      </c>
-      <c r="I12">
-        <v>100</v>
+        <v>102.2</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3158,29 +4446,29 @@
         <v>3</v>
       </c>
       <c r="B13">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="C13">
-        <v>61239</v>
+        <v>108</v>
       </c>
       <c r="D13">
-        <v>75965</v>
+        <v>153</v>
       </c>
       <c r="E13">
-        <v>73963</v>
+        <v>561</v>
       </c>
       <c r="F13">
-        <v>71925</v>
+        <v>118</v>
       </c>
       <c r="G13">
-        <v>66106</v>
+        <v>110</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>69839.600000000006</v>
-      </c>
-      <c r="I13">
-        <v>100</v>
+        <v>210</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3188,29 +4476,29 @@
         <v>3</v>
       </c>
       <c r="B14">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C14">
-        <v>373</v>
+        <v>299</v>
       </c>
       <c r="D14">
-        <v>308</v>
+        <v>598</v>
       </c>
       <c r="E14">
-        <v>163</v>
+        <v>431</v>
       </c>
       <c r="F14">
-        <v>123</v>
+        <v>232</v>
       </c>
       <c r="G14">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>217.2</v>
-      </c>
-      <c r="I14">
-        <v>500</v>
+        <v>356.4</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3218,29 +4506,29 @@
         <v>3</v>
       </c>
       <c r="B15">
-        <v>200</v>
+        <v>5000</v>
       </c>
       <c r="C15">
-        <v>318</v>
+        <v>1055</v>
       </c>
       <c r="D15">
-        <v>115</v>
+        <v>697</v>
       </c>
       <c r="E15">
-        <v>91</v>
+        <v>555</v>
       </c>
       <c r="F15">
-        <v>90</v>
+        <v>1076</v>
       </c>
       <c r="G15">
-        <v>84</v>
+        <v>606</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>139.6</v>
-      </c>
-      <c r="I15">
-        <v>500</v>
+        <v>797.8</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3248,29 +4536,29 @@
         <v>3</v>
       </c>
       <c r="B16">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="C16">
-        <v>661</v>
+        <v>2396</v>
       </c>
       <c r="D16">
-        <v>519</v>
+        <v>2101</v>
       </c>
       <c r="E16">
-        <v>510</v>
+        <v>1725</v>
       </c>
       <c r="F16">
-        <v>524</v>
+        <v>1989</v>
       </c>
       <c r="G16">
-        <v>475</v>
+        <v>2017</v>
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>537.79999999999995</v>
-      </c>
-      <c r="I16">
-        <v>500</v>
+        <v>2045.6</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3278,29 +4566,29 @@
         <v>3</v>
       </c>
       <c r="B17">
-        <v>1000</v>
+        <v>50000</v>
       </c>
       <c r="C17">
-        <v>2207</v>
+        <v>4276</v>
       </c>
       <c r="D17">
-        <v>1479</v>
+        <v>3089</v>
       </c>
       <c r="E17">
-        <v>1319</v>
+        <v>4841</v>
       </c>
       <c r="F17">
-        <v>964</v>
+        <v>3756</v>
       </c>
       <c r="G17">
-        <v>913</v>
+        <v>4303</v>
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>1376.4</v>
-      </c>
-      <c r="I17">
-        <v>500</v>
+        <v>4053</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3308,29 +4596,29 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <v>5000</v>
+        <v>100000</v>
       </c>
       <c r="C18">
-        <v>15050</v>
+        <v>7264</v>
       </c>
       <c r="D18">
-        <v>14734</v>
+        <v>7259</v>
       </c>
       <c r="E18">
-        <v>11741</v>
+        <v>11465</v>
       </c>
       <c r="F18">
-        <v>11328</v>
+        <v>6389</v>
       </c>
       <c r="G18">
-        <v>11589</v>
+        <v>7990</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
-        <v>12888.4</v>
-      </c>
-      <c r="I18">
-        <v>500</v>
+        <v>8073.4</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3338,29 +4626,29 @@
         <v>3</v>
       </c>
       <c r="B19">
-        <v>10000</v>
+        <v>500000</v>
       </c>
       <c r="C19">
-        <v>42163</v>
+        <v>48024</v>
       </c>
       <c r="D19">
-        <v>45384</v>
+        <v>58624</v>
       </c>
       <c r="E19">
-        <v>45710</v>
+        <v>49068</v>
       </c>
       <c r="F19">
-        <v>45193</v>
+        <v>45919</v>
       </c>
       <c r="G19">
-        <v>49007</v>
+        <v>36539</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>45491.4</v>
-      </c>
-      <c r="I19">
-        <v>500</v>
+        <v>47634.8</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3368,28 +4656,28 @@
         <v>3</v>
       </c>
       <c r="B20">
-        <v>100</v>
+        <v>1000000</v>
       </c>
       <c r="C20">
-        <v>365</v>
+        <v>100684</v>
       </c>
       <c r="D20">
-        <v>450</v>
+        <v>74499</v>
       </c>
       <c r="E20">
-        <v>119</v>
+        <v>80580</v>
       </c>
       <c r="F20">
-        <v>121</v>
+        <v>68815</v>
       </c>
       <c r="G20">
-        <v>94</v>
+        <v>80626</v>
       </c>
       <c r="H20">
         <f t="shared" si="0"/>
-        <v>229.8</v>
-      </c>
-      <c r="I20">
+        <v>81040.800000000003</v>
+      </c>
+      <c r="I20" s="1">
         <v>1000</v>
       </c>
     </row>
@@ -3398,28 +4686,28 @@
         <v>3</v>
       </c>
       <c r="B21">
-        <v>200</v>
+        <v>2000000</v>
       </c>
       <c r="C21">
-        <v>230</v>
+        <v>162146</v>
       </c>
       <c r="D21">
-        <v>206</v>
+        <v>177077</v>
       </c>
       <c r="E21">
-        <v>105</v>
+        <v>142111</v>
       </c>
       <c r="F21">
-        <v>94</v>
+        <v>169582</v>
       </c>
       <c r="G21">
-        <v>91</v>
+        <v>144546</v>
       </c>
       <c r="H21">
         <f t="shared" si="0"/>
-        <v>145.19999999999999</v>
-      </c>
-      <c r="I21">
+        <v>159092.4</v>
+      </c>
+      <c r="I21" s="1">
         <v>1000</v>
       </c>
     </row>
@@ -3428,29 +4716,29 @@
         <v>3</v>
       </c>
       <c r="B22">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="C22">
-        <v>487</v>
+        <v>16</v>
       </c>
       <c r="D22">
-        <v>490</v>
+        <v>23</v>
       </c>
       <c r="E22">
-        <v>722</v>
+        <v>19</v>
       </c>
       <c r="F22">
-        <v>523</v>
+        <v>18</v>
       </c>
       <c r="G22">
-        <v>486</v>
+        <v>20</v>
       </c>
       <c r="H22">
-        <f t="shared" si="0"/>
-        <v>541.6</v>
+        <f>AVERAGE(C22:G22)</f>
+        <v>19.2</v>
       </c>
       <c r="I22">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3458,29 +4746,29 @@
         <v>3</v>
       </c>
       <c r="B23">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C23">
-        <v>888</v>
+        <v>111</v>
       </c>
       <c r="D23">
-        <v>721</v>
+        <v>115</v>
       </c>
       <c r="E23">
-        <v>665</v>
+        <v>105</v>
       </c>
       <c r="F23">
-        <v>753</v>
+        <v>109</v>
       </c>
       <c r="G23">
-        <v>665</v>
+        <v>107</v>
       </c>
       <c r="H23">
-        <f t="shared" si="0"/>
-        <v>738.4</v>
+        <f>AVERAGE(C23:G23)</f>
+        <v>109.4</v>
       </c>
       <c r="I23">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3488,29 +4776,29 @@
         <v>3</v>
       </c>
       <c r="B24">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="C24">
-        <v>12572</v>
+        <v>308</v>
       </c>
       <c r="D24">
-        <v>13146</v>
+        <v>232</v>
       </c>
       <c r="E24">
-        <v>17757</v>
+        <v>225</v>
       </c>
       <c r="F24">
-        <v>15955</v>
+        <v>309</v>
       </c>
       <c r="G24">
-        <v>10429</v>
+        <v>225</v>
       </c>
       <c r="H24">
-        <f t="shared" si="0"/>
-        <v>13971.8</v>
+        <f>AVERAGE(C24:G24)</f>
+        <v>259.8</v>
       </c>
       <c r="I24">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3518,29 +4806,509 @@
         <v>3</v>
       </c>
       <c r="B25">
+        <v>5000</v>
+      </c>
+      <c r="C25">
+        <v>963</v>
+      </c>
+      <c r="D25">
+        <v>895</v>
+      </c>
+      <c r="E25">
+        <v>1516</v>
+      </c>
+      <c r="F25">
+        <v>1531</v>
+      </c>
+      <c r="G25">
+        <v>1374</v>
+      </c>
+      <c r="H25">
+        <f>AVERAGE(C25:G25)</f>
+        <v>1255.8</v>
+      </c>
+      <c r="I25">
         <v>10000</v>
       </c>
-      <c r="C25">
-        <v>40335</v>
-      </c>
-      <c r="D25">
-        <v>40087</v>
-      </c>
-      <c r="E25">
-        <v>39959</v>
-      </c>
-      <c r="F25">
-        <v>40528</v>
-      </c>
-      <c r="G25">
-        <v>42497</v>
-      </c>
-      <c r="H25">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>10000</v>
+      </c>
+      <c r="C26">
+        <v>5022</v>
+      </c>
+      <c r="D26">
+        <v>2404</v>
+      </c>
+      <c r="E26">
+        <v>3895</v>
+      </c>
+      <c r="F26">
+        <v>2119</v>
+      </c>
+      <c r="G26">
+        <v>2448</v>
+      </c>
+      <c r="H26">
+        <f>AVERAGE(C26:G26)</f>
+        <v>3177.6</v>
+      </c>
+      <c r="I26">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>50000</v>
+      </c>
+      <c r="C27">
+        <v>4762</v>
+      </c>
+      <c r="D27">
+        <v>7865</v>
+      </c>
+      <c r="E27">
+        <v>3235</v>
+      </c>
+      <c r="F27">
+        <v>7770</v>
+      </c>
+      <c r="G27">
+        <v>4342</v>
+      </c>
+      <c r="H27">
+        <f>AVERAGE(C27:G27)</f>
+        <v>5594.8</v>
+      </c>
+      <c r="I27">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>100000</v>
+      </c>
+      <c r="C28">
+        <v>9895</v>
+      </c>
+      <c r="D28">
+        <v>7938</v>
+      </c>
+      <c r="E28">
+        <v>6091</v>
+      </c>
+      <c r="F28">
+        <v>8210</v>
+      </c>
+      <c r="G28">
+        <v>9572</v>
+      </c>
+      <c r="H28">
+        <f>AVERAGE(C28:G28)</f>
+        <v>8341.2000000000007</v>
+      </c>
+      <c r="I28">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>500000</v>
+      </c>
+      <c r="C29">
+        <v>35705</v>
+      </c>
+      <c r="D29">
+        <v>31844</v>
+      </c>
+      <c r="E29">
+        <v>33569</v>
+      </c>
+      <c r="F29">
+        <v>39872</v>
+      </c>
+      <c r="G29">
+        <v>43711</v>
+      </c>
+      <c r="H29">
+        <f>AVERAGE(C29:G29)</f>
+        <v>36940.199999999997</v>
+      </c>
+      <c r="I29">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>1000000</v>
+      </c>
+      <c r="C30">
+        <v>107692</v>
+      </c>
+      <c r="D30">
+        <v>81985</v>
+      </c>
+      <c r="E30">
+        <v>68246</v>
+      </c>
+      <c r="F30">
+        <v>65854</v>
+      </c>
+      <c r="G30">
+        <v>77149</v>
+      </c>
+      <c r="H30">
+        <f>AVERAGE(C30:G30)</f>
+        <v>80185.2</v>
+      </c>
+      <c r="I30">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>2000000</v>
+      </c>
+      <c r="C31">
+        <v>147631</v>
+      </c>
+      <c r="D31">
+        <v>150644</v>
+      </c>
+      <c r="E31">
+        <v>147006</v>
+      </c>
+      <c r="F31">
+        <v>159424</v>
+      </c>
+      <c r="G31">
+        <v>138692</v>
+      </c>
+      <c r="H31">
+        <f>AVERAGE(C31:G31)</f>
+        <v>148679.4</v>
+      </c>
+      <c r="I31">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <v>100</v>
+      </c>
+      <c r="C32">
+        <v>117</v>
+      </c>
+      <c r="D32">
+        <v>115</v>
+      </c>
+      <c r="E32">
+        <v>122</v>
+      </c>
+      <c r="F32">
+        <v>101</v>
+      </c>
+      <c r="G32">
+        <v>104</v>
+      </c>
+      <c r="H32">
         <f t="shared" si="0"/>
-        <v>40681.199999999997</v>
-      </c>
-      <c r="I25">
+        <v>111.8</v>
+      </c>
+      <c r="I32">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>500</v>
+      </c>
+      <c r="C33">
+        <v>180</v>
+      </c>
+      <c r="D33">
+        <v>106</v>
+      </c>
+      <c r="E33">
+        <v>103</v>
+      </c>
+      <c r="F33">
+        <v>106</v>
+      </c>
+      <c r="G33">
+        <v>180</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="I33">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34">
         <v>1000</v>
+      </c>
+      <c r="C34">
+        <v>306</v>
+      </c>
+      <c r="D34">
+        <v>221</v>
+      </c>
+      <c r="E34">
+        <v>220</v>
+      </c>
+      <c r="F34">
+        <v>1779</v>
+      </c>
+      <c r="G34">
+        <v>221</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>549.4</v>
+      </c>
+      <c r="I34">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>5000</v>
+      </c>
+      <c r="C35">
+        <v>856</v>
+      </c>
+      <c r="D35">
+        <v>878</v>
+      </c>
+      <c r="E35">
+        <v>836</v>
+      </c>
+      <c r="F35">
+        <v>930</v>
+      </c>
+      <c r="G35">
+        <v>934</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>886.8</v>
+      </c>
+      <c r="I35">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>10000</v>
+      </c>
+      <c r="C36">
+        <v>1923</v>
+      </c>
+      <c r="D36">
+        <v>1983</v>
+      </c>
+      <c r="E36">
+        <v>3550</v>
+      </c>
+      <c r="F36">
+        <v>1828</v>
+      </c>
+      <c r="G36">
+        <v>1912</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>2239.1999999999998</v>
+      </c>
+      <c r="I36">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>50000</v>
+      </c>
+      <c r="C37">
+        <v>8488</v>
+      </c>
+      <c r="D37">
+        <v>7345</v>
+      </c>
+      <c r="E37">
+        <v>8053</v>
+      </c>
+      <c r="F37">
+        <v>7419</v>
+      </c>
+      <c r="G37">
+        <v>8468</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>7954.6</v>
+      </c>
+      <c r="I37">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>100000</v>
+      </c>
+      <c r="C38">
+        <v>15975</v>
+      </c>
+      <c r="D38">
+        <v>18105</v>
+      </c>
+      <c r="E38">
+        <v>17351</v>
+      </c>
+      <c r="F38">
+        <v>16424</v>
+      </c>
+      <c r="G38">
+        <v>16536</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>16878.2</v>
+      </c>
+      <c r="I38">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>500000</v>
+      </c>
+      <c r="C39">
+        <v>44248</v>
+      </c>
+      <c r="D39">
+        <v>51397</v>
+      </c>
+      <c r="E39">
+        <v>34289</v>
+      </c>
+      <c r="F39">
+        <v>40461</v>
+      </c>
+      <c r="G39">
+        <v>34384</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>40955.800000000003</v>
+      </c>
+      <c r="I39">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>1000000</v>
+      </c>
+      <c r="C40">
+        <v>76532</v>
+      </c>
+      <c r="D40">
+        <v>77822</v>
+      </c>
+      <c r="E40">
+        <v>86568</v>
+      </c>
+      <c r="F40">
+        <v>76668</v>
+      </c>
+      <c r="G40">
+        <v>71413</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="0"/>
+        <v>77800.600000000006</v>
+      </c>
+      <c r="I40">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>2000000</v>
+      </c>
+      <c r="C41">
+        <v>132681</v>
+      </c>
+      <c r="D41">
+        <v>148129</v>
+      </c>
+      <c r="E41">
+        <v>148404</v>
+      </c>
+      <c r="F41">
+        <v>151728</v>
+      </c>
+      <c r="G41">
+        <v>144310</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>145050.4</v>
+      </c>
+      <c r="I41">
+        <v>100000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>